<commit_message>
Update review sheet of SRS
</commit_message>
<xml_diff>
--- a/Software Specification/SRS_Review.xlsx
+++ b/Software Specification/SRS_Review.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="46">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -125,9 +125,6 @@
   </si>
   <si>
     <t>TSH</t>
-  </si>
-  <si>
-    <t>1.0</t>
   </si>
   <si>
     <t>SRS</t>
@@ -180,6 +177,9 @@
   </si>
   <si>
     <t xml:space="preserve">SRS </t>
+  </si>
+  <si>
+    <t>V1.0</t>
   </si>
 </sst>
 </file>
@@ -553,12 +553,39 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -573,33 +600,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -725,7 +725,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -760,7 +760,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -947,7 +947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -958,206 +958,189 @@
   <sheetData>
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33" t="s">
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="39"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="37"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="40"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="37"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="40"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="32"/>
     </row>
     <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="25">
+      <c r="C7" s="26"/>
+      <c r="D7" s="31">
         <v>1</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="26"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="32"/>
     </row>
     <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="25" t="s">
+      <c r="C8" s="26"/>
+      <c r="D8" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="32"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="25" t="s">
+      <c r="C9" s="26"/>
+      <c r="D9" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="26"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="32"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="29"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="31"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="40"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="36"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35" t="s">
+      <c r="D12" s="34"/>
+      <c r="E12" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35" t="s">
+      <c r="F12" s="34"/>
+      <c r="G12" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="36"/>
+      <c r="H12" s="35"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25" t="s">
+      <c r="D13" s="31"/>
+      <c r="E13" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25" t="s">
+      <c r="F13" s="31"/>
+      <c r="G13" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="26"/>
+      <c r="H13" s="32"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="26"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="32"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="26"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="32"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="26"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="32"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="26"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="32"/>
     </row>
     <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="28"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1174,6 +1157,23 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1184,8 +1184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1238,16 +1238,16 @@
         <v>34</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>36</v>
       </c>
       <c r="E2" s="8">
         <v>1</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10" t="s">
@@ -1256,15 +1256,23 @@
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="7"/>
+      <c r="A3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="E3" s="8" t="s">
         <v>31</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10" t="s">
@@ -1276,15 +1284,23 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="7"/>
+      <c r="A4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="E4" s="8" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="10" t="s">
@@ -1296,15 +1312,23 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="7"/>
+      <c r="A5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="E5" s="8" t="s">
         <v>32</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10" t="s">
@@ -1313,15 +1337,23 @@
       <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="7"/>
+      <c r="A6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="E6" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>41</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>42</v>
       </c>
       <c r="G6" s="10"/>
       <c r="H6" s="10" t="s">
@@ -1333,15 +1365,23 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="7"/>
+      <c r="A7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="E7" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="10" t="s">
@@ -1353,15 +1393,23 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="7"/>
+      <c r="A8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="E8" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10" t="s">

</xml_diff>